<commit_message>
fixed a small issue relating to the excel exporter
</commit_message>
<xml_diff>
--- a/src/main/java/GUI/resources/ExportedGradeData.xlsx
+++ b/src/main/java/GUI/resources/ExportedGradeData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="CS 3398" r:id="rId5" sheetId="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="51">
   <si>
     <t>School</t>
   </si>

</xml_diff>